<commit_message>
Send mails to users every day
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>name</t>
   </si>
@@ -45,7 +45,7 @@
         <rFont val="Helvetica Neue"/>
         <family val="2"/>
       </rPr>
-      <t>ypddjuio@yomail.info</t>
+      <t>08jccpq330@spymail.one</t>
     </r>
   </si>
   <si>
@@ -66,11 +66,11 @@
         <rFont val="Helvetica Neue"/>
         <family val="2"/>
       </rPr>
-      <t>kawnlyiw@supere.ml</t>
+      <t>akkpeouddbvatl@dropmail.me</t>
     </r>
   </si>
   <si>
-    <t>nasa</t>
+    <t>python</t>
   </si>
   <si>
     <t>Sim</t>
@@ -90,8 +90,23 @@
         <rFont val="Helvetica Neue"/>
         <family val="2"/>
       </rPr>
-      <t>pythonprocourse2@gmail.com</t>
+      <t>akkpeoomwzokhy@dropmail.me</t>
     </r>
+  </si>
+  <si>
+    <t>nasa</t>
+  </si>
+  <si>
+    <t>Ivanna</t>
+  </si>
+  <si>
+    <t>Parf</t>
+  </si>
+  <si>
+    <t>mainpy571@gmail.com</t>
+  </si>
+  <si>
+    <t>yoga</t>
   </si>
 </sst>
 </file>
@@ -115,7 +130,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -412,36 +427,36 @@
   </cellStyleXfs>
   <cellXfs count="20">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="9" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -467,7 +482,7 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -784,102 +799,110 @@
     <col min="5" max="5" style="19" width="8.290714285714287" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18">
-      <c r="A1" s="1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="29.25">
-      <c r="A2" s="3" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="6"/>
+      <c r="E2" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18">
-      <c r="A3" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="1">
+      <c r="A3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="6"/>
+      <c r="E3" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="29.25">
-      <c r="A4" s="7" t="s">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="31.5" customFormat="1" s="1">
+      <c r="A4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="6"/>
+      <c r="D4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="7"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18" customFormat="1" s="10">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="1">
+      <c r="A5" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="E5" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25" customFormat="1" s="10">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A6" s="14"/>
       <c r="B6" s="15"/>
       <c r="C6" s="15"/>
       <c r="D6" s="15"/>
       <c r="E6" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25" customFormat="1" s="10">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
       <c r="E7" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="17.25" customFormat="1" s="10">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A8" s="14"/>
       <c r="B8" s="15"/>
       <c r="C8" s="15"/>
       <c r="D8" s="15"/>
       <c r="E8" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="17.25" customFormat="1" s="10">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A9" s="14"/>
       <c r="B9" s="15"/>
       <c r="C9" s="15"/>
       <c r="D9" s="15"/>
       <c r="E9" s="13"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="17.25" customFormat="1" s="10">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="1">
       <c r="A10" s="16"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>

</xml_diff>